<commit_message>
Committing of Other Tahsil and Forward Back to Parent Tahsil Code
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testData.xlsx
+++ b/src/test/resources/excel/testData.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\workspace\Framework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B2498E-A745-4921-B426-CF16B82ACC85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BCF45C-D268-4CAF-AE70-EF245CFAA6D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Runner" sheetId="1" r:id="rId1"/>
-    <sheet name="data" sheetId="2" r:id="rId2"/>
+    <sheet name="LegalHeir" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,69 +25,141 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
-  <si>
-    <t>testname</t>
-  </si>
-  <si>
-    <t>testdescription</t>
-  </si>
-  <si>
-    <t>execute</t>
-  </si>
-  <si>
-    <t>priority</t>
-  </si>
-  <si>
-    <t>count</t>
-  </si>
-  <si>
-    <t>logintest</t>
-  </si>
-  <si>
-    <t>to check login and logout</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>newtest</t>
-  </si>
-  <si>
-    <t>some new test</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>csc1.sundar</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+  <si>
+    <t>tdr.bargarh</t>
+  </si>
+  <si>
+    <t>DeceasedPerson</t>
+  </si>
+  <si>
+    <t>DeceasedFather</t>
+  </si>
+  <si>
+    <t>Relationship</t>
+  </si>
+  <si>
+    <t>Sunil@123</t>
+  </si>
+  <si>
+    <t>rakesh</t>
+  </si>
+  <si>
+    <t>ramesh</t>
+  </si>
+  <si>
+    <t>Father</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>DeathPlace</t>
+  </si>
+  <si>
+    <t>bangalore</t>
+  </si>
+  <si>
+    <t>DeathAddress</t>
+  </si>
+  <si>
+    <t>Legalname</t>
+  </si>
+  <si>
+    <t>Legalage</t>
+  </si>
+  <si>
+    <t>LegalmartialStatus</t>
+  </si>
+  <si>
+    <t>ganesh</t>
+  </si>
+  <si>
+    <t>Unmarried</t>
+  </si>
+  <si>
+    <t>RelationshipDeceased</t>
+  </si>
+  <si>
+    <t>some</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>some reason</t>
+  </si>
+  <si>
+    <t>Pdistrict</t>
+  </si>
+  <si>
+    <t>Ptahsil</t>
+  </si>
+  <si>
+    <t>Psubdivision</t>
+  </si>
+  <si>
+    <t>Pri</t>
+  </si>
+  <si>
+    <t>Pvillage</t>
+  </si>
+  <si>
+    <t>Bargarh</t>
+  </si>
+  <si>
+    <t>Jamurda</t>
+  </si>
+  <si>
+    <t>jamu</t>
+  </si>
+  <si>
+    <t>Ppolicestation</t>
+  </si>
+  <si>
+    <t>some station</t>
+  </si>
+  <si>
+    <t>Place</t>
+  </si>
+  <si>
+    <t>some place</t>
+  </si>
+  <si>
+    <t>OfficialDA</t>
+  </si>
+  <si>
+    <t>da.bargarh</t>
+  </si>
+  <si>
+    <t>OfficialRI</t>
+  </si>
+  <si>
+    <t>ri.jamurda</t>
+  </si>
+  <si>
+    <t>OfficialTahsil</t>
+  </si>
+  <si>
+    <t>Portalemailaddress</t>
+  </si>
+  <si>
+    <t>Portalpassword</t>
+  </si>
+  <si>
+    <t>sunnyxmail@gmail.com</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
   <si>
     <t>Pass@1231</t>
-  </si>
-  <si>
-    <t>tdr.bargarh</t>
-  </si>
-  <si>
-    <t>browser</t>
-  </si>
-  <si>
-    <t>chrome</t>
-  </si>
-  <si>
-    <t>firefox</t>
-  </si>
-  <si>
-    <t>Pass@123</t>
   </si>
 </sst>
 </file>
@@ -417,163 +488,195 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0DD2077-59A3-4AEA-AE73-174C5ECD4E74}">
+  <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>23</v>
+      </c>
+      <c r="U1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" t="s">
+        <v>30</v>
+      </c>
+      <c r="X1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R2" t="s">
+        <v>27</v>
+      </c>
+      <c r="S2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U2" t="s">
+        <v>28</v>
+      </c>
+      <c r="V2" t="s">
+        <v>29</v>
+      </c>
+      <c r="W2" t="s">
+        <v>31</v>
+      </c>
+      <c r="X2" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="I3" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0DD2077-59A3-4AEA-AE73-174C5ECD4E74}">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>15</v>
-      </c>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="I4" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" xr:uid="{BE711F93-0C03-4B35-B48F-1BB78AFC9EBD}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{6635DACB-BB70-45D0-BB6E-B41865A4EA1F}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{28EF5963-9C68-49AE-8B6A-3EB8827F1492}"/>
+    <hyperlink ref="I2" r:id="rId1" display="Pass@123" xr:uid="{6635DACB-BB70-45D0-BB6E-B41865A4EA1F}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{C1C766DB-DBC6-4F89-8F77-9D14AC945A0C}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{420A93CB-B0E8-41AD-82CB-630474291E60}"/>
+    <hyperlink ref="D2" r:id="rId4" xr:uid="{7EC2DD05-2788-400A-990C-3BD6CE096500}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Committing of reading the data from excel for 10 Services
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testData.xlsx
+++ b/src/test/resources/excel/testData.xlsx
@@ -8,12 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\workspace\Framework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BCF45C-D268-4CAF-AE70-EF245CFAA6D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA35BF67-4DAE-4305-B50A-AFF86B3AEECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LegalHeir" sheetId="2" r:id="rId1"/>
+    <sheet name="Resident" sheetId="3" r:id="rId2"/>
+    <sheet name="Solvency" sheetId="4" r:id="rId3"/>
+    <sheet name="Ror" sheetId="5" r:id="rId4"/>
+    <sheet name="Income" sheetId="6" r:id="rId5"/>
+    <sheet name="Incomeandasset" sheetId="7" r:id="rId6"/>
+    <sheet name="Guardian" sheetId="8" r:id="rId7"/>
+    <sheet name="Caste" sheetId="9" r:id="rId8"/>
+    <sheet name="Tribe" sheetId="10" r:id="rId9"/>
+    <sheet name="Obc" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="178">
   <si>
     <t>tdr.bargarh</t>
   </si>
@@ -160,6 +169,405 @@
   </si>
   <si>
     <t>Pass@1231</t>
+  </si>
+  <si>
+    <t>Years</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Months</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>some purpose</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>LandPropertyvalue</t>
+  </si>
+  <si>
+    <t>BuildingPropertyValue</t>
+  </si>
+  <si>
+    <t>OtherImmovableProperty</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>ImmovableProperty</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>Rdistrict</t>
+  </si>
+  <si>
+    <t>Rsubdivision</t>
+  </si>
+  <si>
+    <t>Rtahsil</t>
+  </si>
+  <si>
+    <t>Rri</t>
+  </si>
+  <si>
+    <t>Rvillage</t>
+  </si>
+  <si>
+    <t>Rpolicestation</t>
+  </si>
+  <si>
+    <t>Khatano</t>
+  </si>
+  <si>
+    <t>Plotno</t>
+  </si>
+  <si>
+    <t>2002/20</t>
+  </si>
+  <si>
+    <t>Caste</t>
+  </si>
+  <si>
+    <t>some caste</t>
+  </si>
+  <si>
+    <t>Agriculture</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>Trade</t>
+  </si>
+  <si>
+    <t>Othersources</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Sname</t>
+  </si>
+  <si>
+    <t>Sage</t>
+  </si>
+  <si>
+    <t>Sgender</t>
+  </si>
+  <si>
+    <t>Srelation</t>
+  </si>
+  <si>
+    <t>kumar</t>
+  </si>
+  <si>
+    <t>Brother</t>
+  </si>
+  <si>
+    <t>Cname</t>
+  </si>
+  <si>
+    <t>Cage</t>
+  </si>
+  <si>
+    <t>Cgender</t>
+  </si>
+  <si>
+    <t>Crelation</t>
+  </si>
+  <si>
+    <t>ram</t>
+  </si>
+  <si>
+    <t>Son</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Profession</t>
+  </si>
+  <si>
+    <t>Pleasespecify</t>
+  </si>
+  <si>
+    <t>Othersourcesincome</t>
+  </si>
+  <si>
+    <t>Asset</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>some location</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>Agricultural Land</t>
+  </si>
+  <si>
+    <t>in Acre</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Legalprefix</t>
+  </si>
+  <si>
+    <t>Legalfirstname</t>
+  </si>
+  <si>
+    <t>Legallastname</t>
+  </si>
+  <si>
+    <t>Legalffirstname</t>
+  </si>
+  <si>
+    <t>Ldistrict</t>
+  </si>
+  <si>
+    <t>Lsubdivision</t>
+  </si>
+  <si>
+    <t>Ltahsil</t>
+  </si>
+  <si>
+    <t>Lri</t>
+  </si>
+  <si>
+    <t>Lvillage</t>
+  </si>
+  <si>
+    <t>Lpolicestation</t>
+  </si>
+  <si>
+    <t>Relation</t>
+  </si>
+  <si>
+    <t>Shri</t>
+  </si>
+  <si>
+    <t>Mano</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>vijay</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>poluce</t>
+  </si>
+  <si>
+    <t>Aunt</t>
+  </si>
+  <si>
+    <t>someplace</t>
+  </si>
+  <si>
+    <t>Religion</t>
+  </si>
+  <si>
+    <t>Gandia</t>
+  </si>
+  <si>
+    <t>Hindu</t>
+  </si>
+  <si>
+    <t>Tribe</t>
+  </si>
+  <si>
+    <t>Sabara</t>
+  </si>
+  <si>
+    <t>Perdistrict</t>
+  </si>
+  <si>
+    <t>Pervillage</t>
+  </si>
+  <si>
+    <t>Perblock</t>
+  </si>
+  <si>
+    <t>Pergp</t>
+  </si>
+  <si>
+    <t>Predistrict</t>
+  </si>
+  <si>
+    <t>Preblock</t>
+  </si>
+  <si>
+    <t>Pregp</t>
+  </si>
+  <si>
+    <t>Previllage</t>
+  </si>
+  <si>
+    <t>Designation</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>Govdesignation</t>
+  </si>
+  <si>
+    <t>Govscaleofpay</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>InterOrganization</t>
+  </si>
+  <si>
+    <t>Interdesignation</t>
+  </si>
+  <si>
+    <t>PubOrganization</t>
+  </si>
+  <si>
+    <t>Pubdesignation</t>
+  </si>
+  <si>
+    <t>Annualincome</t>
+  </si>
+  <si>
+    <t>Paradesignation</t>
+  </si>
+  <si>
+    <t>ParaScaleofpay</t>
+  </si>
+  <si>
+    <t>Appoccupation</t>
+  </si>
+  <si>
+    <t>Proplocation</t>
+  </si>
+  <si>
+    <t>Propsize</t>
+  </si>
+  <si>
+    <t>Irrigatedone</t>
+  </si>
+  <si>
+    <t>Irrigatedtwo</t>
+  </si>
+  <si>
+    <t>Irrigatedthree</t>
+  </si>
+  <si>
+    <t>UnirragatedOne</t>
+  </si>
+  <si>
+    <t>Unirragatedtwo</t>
+  </si>
+  <si>
+    <t>Unirragatedthree</t>
+  </si>
+  <si>
+    <t>Crops</t>
+  </si>
+  <si>
+    <t>Areaofplantation</t>
+  </si>
+  <si>
+    <t>Locationofproperty</t>
+  </si>
+  <si>
+    <t>Detailsofproperty</t>
+  </si>
+  <si>
+    <t>Use</t>
+  </si>
+  <si>
+    <t>Wealthannualincome</t>
+  </si>
+  <si>
+    <t>Wealthtaxdetails</t>
+  </si>
+  <si>
+    <t>remarks</t>
+  </si>
+  <si>
+    <t>Balangir</t>
+  </si>
+  <si>
+    <t>Adendungri</t>
+  </si>
+  <si>
+    <t>Agharia</t>
+  </si>
+  <si>
+    <t>Desi</t>
+  </si>
+  <si>
+    <t>Central</t>
+  </si>
+  <si>
+    <t>SRIT</t>
+  </si>
+  <si>
+    <t>designation</t>
+  </si>
+  <si>
+    <t>1999</t>
+  </si>
+  <si>
+    <t>tsting</t>
+  </si>
+  <si>
+    <t>78</t>
+  </si>
+  <si>
+    <t>one</t>
+  </si>
+  <si>
+    <t>two</t>
+  </si>
+  <si>
+    <t>thre</t>
+  </si>
+  <si>
+    <t>Crop plant</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>13</t>
   </si>
 </sst>
 </file>
@@ -491,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0DD2077-59A3-4AEA-AE73-174C5ECD4E74}">
   <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,4 +1087,1743 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA65B40-FE79-4E48-A903-52D74A50D628}">
+  <dimension ref="A1:BB2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="AO1" workbookViewId="0">
+      <selection activeCell="AW9" sqref="AW9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="41" width="12" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="15" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="6" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="18.28515625" customWidth="1"/>
+    <col min="51" max="51" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="8.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" t="s">
+        <v>125</v>
+      </c>
+      <c r="P1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>128</v>
+      </c>
+      <c r="R1" t="s">
+        <v>126</v>
+      </c>
+      <c r="S1" t="s">
+        <v>129</v>
+      </c>
+      <c r="T1" t="s">
+        <v>130</v>
+      </c>
+      <c r="U1" t="s">
+        <v>131</v>
+      </c>
+      <c r="V1" t="s">
+        <v>132</v>
+      </c>
+      <c r="W1" t="s">
+        <v>67</v>
+      </c>
+      <c r="X1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>133</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>134</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>136</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>141</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>158</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>157</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>159</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>160</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N2" t="s">
+        <v>119</v>
+      </c>
+      <c r="O2" t="s">
+        <v>162</v>
+      </c>
+      <c r="P2" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>162</v>
+      </c>
+      <c r="R2" t="s">
+        <v>163</v>
+      </c>
+      <c r="S2" t="s">
+        <v>162</v>
+      </c>
+      <c r="T2" t="s">
+        <v>162</v>
+      </c>
+      <c r="U2" t="s">
+        <v>162</v>
+      </c>
+      <c r="V2" t="s">
+        <v>163</v>
+      </c>
+      <c r="W2" t="s">
+        <v>164</v>
+      </c>
+      <c r="X2" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>165</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>133</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC2">
+        <v>23</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>167</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>168</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>167</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>168</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>168</v>
+      </c>
+      <c r="AJ2">
+        <v>1000</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>170</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>172</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>173</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>174</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AR2" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="AS2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>175</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AV2" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AZ2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>96</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{68A61DFC-2943-48E2-B05B-EAF6039E6274}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{72AE3D8F-0591-4947-A002-850F2A70D025}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{46D4F354-67E1-4A57-AA7D-19B9C6583487}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8066D58A-F9A7-4841-850D-25A40E944F2F}">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:U2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="14.85546875" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" t="s">
+        <v>49</v>
+      </c>
+      <c r="P2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{BAF0C683-58D0-4290-906E-D245BA5C0232}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{44B74987-7E7A-4E67-B9CC-CE8C6FAAF157}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{CD6B2FB7-DFCB-4E4A-B7A6-D010F4C02606}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2C77AFB-ECB8-4E38-B8AF-1609FF544C4D}">
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>52</v>
+      </c>
+      <c r="R1" t="s">
+        <v>53</v>
+      </c>
+      <c r="S1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="R2" t="s">
+        <v>54</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{467AB7EB-C352-4A89-AB73-ACA612BBF23B}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{72DC759D-FF2A-493F-8A24-EA5EFA88DD26}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{65F97CF0-7AEF-463C-A599-9E5C19A3D862}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63A03D48-B6EA-4659-89E6-F7F49F374668}">
+  <dimension ref="A1:W2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:N2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>60</v>
+      </c>
+      <c r="R1" t="s">
+        <v>61</v>
+      </c>
+      <c r="S1" t="s">
+        <v>62</v>
+      </c>
+      <c r="T1" t="s">
+        <v>63</v>
+      </c>
+      <c r="U1" t="s">
+        <v>64</v>
+      </c>
+      <c r="V1" t="s">
+        <v>65</v>
+      </c>
+      <c r="W1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>27</v>
+      </c>
+      <c r="R2" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T2" t="s">
+        <v>31</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="W2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{9319E01F-6DBC-414C-AAFA-21A3309DC606}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{854FEE53-8130-4EA2-8AA3-4443BD736B50}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{41109380-70C1-443D-993B-382C27742136}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C8F8FDE-4D94-4CE3-A898-5A5818BAD9EC}">
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:N1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>71</v>
+      </c>
+      <c r="R1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{34DE0E99-CCAE-4976-A387-8F72BE673E10}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{1DE26D99-34BF-4948-B78F-CDBD79A45EB7}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{A66A25C9-1DF2-46D6-A2F7-206D7ECC1ED7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7101295-8A57-4117-B7C0-CB5330BEB457}">
+  <dimension ref="A1:AG2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:N2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" t="s">
+        <v>73</v>
+      </c>
+      <c r="P1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>76</v>
+      </c>
+      <c r="R1" t="s">
+        <v>77</v>
+      </c>
+      <c r="S1" t="s">
+        <v>78</v>
+      </c>
+      <c r="T1" t="s">
+        <v>81</v>
+      </c>
+      <c r="U1" t="s">
+        <v>82</v>
+      </c>
+      <c r="V1" t="s">
+        <v>83</v>
+      </c>
+      <c r="W1" t="s">
+        <v>84</v>
+      </c>
+      <c r="X1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" t="s">
+        <v>74</v>
+      </c>
+      <c r="P2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="R2" t="s">
+        <v>9</v>
+      </c>
+      <c r="S2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T2" t="s">
+        <v>85</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="V2" t="s">
+        <v>9</v>
+      </c>
+      <c r="W2" t="s">
+        <v>86</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>98</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{CFAAE6C5-C62B-438B-9ED6-50C73744E336}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{F8E6A2E6-1E7E-4B96-9272-16E306BD2BB1}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{6E54D1C5-D27F-4FCD-802F-5B7CEE58E1D0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1437BAE-7325-43A0-82A7-C99B55C0E16F}">
+  <dimension ref="A1:AA2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" t="s">
+        <v>101</v>
+      </c>
+      <c r="P1" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>103</v>
+      </c>
+      <c r="R1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" t="s">
+        <v>104</v>
+      </c>
+      <c r="T1" t="s">
+        <v>103</v>
+      </c>
+      <c r="U1" t="s">
+        <v>105</v>
+      </c>
+      <c r="V1" t="s">
+        <v>106</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+      <c r="X1" t="s">
+        <v>108</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" t="s">
+        <v>112</v>
+      </c>
+      <c r="P2" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>114</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S2" t="s">
+        <v>115</v>
+      </c>
+      <c r="T2" t="s">
+        <v>116</v>
+      </c>
+      <c r="U2" t="s">
+        <v>27</v>
+      </c>
+      <c r="V2" t="s">
+        <v>27</v>
+      </c>
+      <c r="W2" t="s">
+        <v>27</v>
+      </c>
+      <c r="X2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{F5E860F9-3F7D-4785-AF4C-3701A73C9320}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{84E35B3A-1810-43DC-83A0-26F78C606103}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{B8600A80-44C7-4F1A-BF13-F773EA9903D4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8EA0402-FFBF-495C-B35C-6EE85853467D}">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:P2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N2" t="s">
+        <v>119</v>
+      </c>
+      <c r="O2" t="s">
+        <v>121</v>
+      </c>
+      <c r="P2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{CBE42E18-73C8-4BAF-98EE-1CBB56E1456F}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{A3163FB7-B6AA-469B-97D3-5FEC40D3A5EF}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{E347ACD5-7329-4DCE-BC68-8148D8E3DC9F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D60BC825-1D6C-4043-8C6F-50F228FFE52E}">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:N2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" t="s">
+        <v>123</v>
+      </c>
+      <c r="P1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N2" t="s">
+        <v>119</v>
+      </c>
+      <c r="O2" t="s">
+        <v>124</v>
+      </c>
+      <c r="P2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{D3FB033C-EEE3-41DE-B033-22123D088E53}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{BE472250-A864-4567-9445-84F46BBD38CA}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{D8ABE86B-7487-4882-87AE-CF4ED9515C81}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
excel data reading and switching to mulitple tabs for all the services
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testData.xlsx
+++ b/src/test/resources/excel/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\workspace\Framework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA35BF67-4DAE-4305-B50A-AFF86B3AEECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA5D1FE-313C-48E3-A01C-2FCEDA8D7FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LegalHeir" sheetId="2" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="Caste" sheetId="9" r:id="rId8"/>
     <sheet name="Tribe" sheetId="10" r:id="rId9"/>
     <sheet name="Obc" sheetId="11" r:id="rId10"/>
+    <sheet name="Sebc" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="178">
   <si>
     <t>tdr.bargarh</t>
   </si>
@@ -1093,8 +1094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA65B40-FE79-4E48-A903-52D74A50D628}">
   <dimension ref="A1:BB2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO1" workbookViewId="0">
-      <selection activeCell="AW9" sqref="AW9"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AB9" sqref="AB9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1402,8 +1403,8 @@
       <c r="AB2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AC2">
-        <v>23</v>
+      <c r="AC2" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="AD2" t="s">
         <v>167</v>
@@ -1486,6 +1487,408 @@
     <hyperlink ref="B2" r:id="rId1" xr:uid="{68A61DFC-2943-48E2-B05B-EAF6039E6274}"/>
     <hyperlink ref="A2" r:id="rId2" xr:uid="{72AE3D8F-0591-4947-A002-850F2A70D025}"/>
     <hyperlink ref="D2" r:id="rId3" xr:uid="{46D4F354-67E1-4A57-AA7D-19B9C6583487}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDCF77BB-4D0A-4A89-8782-127E6C2F1A3E}">
+  <dimension ref="A1:BB2"/>
+  <sheetViews>
+    <sheetView topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AD4" sqref="AD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="41" width="12" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="15" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="8.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" t="s">
+        <v>125</v>
+      </c>
+      <c r="P1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>128</v>
+      </c>
+      <c r="R1" t="s">
+        <v>126</v>
+      </c>
+      <c r="S1" t="s">
+        <v>129</v>
+      </c>
+      <c r="T1" t="s">
+        <v>130</v>
+      </c>
+      <c r="U1" t="s">
+        <v>131</v>
+      </c>
+      <c r="V1" t="s">
+        <v>132</v>
+      </c>
+      <c r="W1" t="s">
+        <v>67</v>
+      </c>
+      <c r="X1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>133</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>134</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>136</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>141</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>158</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>157</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>159</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>160</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N2" t="s">
+        <v>119</v>
+      </c>
+      <c r="O2" t="s">
+        <v>162</v>
+      </c>
+      <c r="P2" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>162</v>
+      </c>
+      <c r="R2" t="s">
+        <v>163</v>
+      </c>
+      <c r="S2" t="s">
+        <v>162</v>
+      </c>
+      <c r="T2" t="s">
+        <v>162</v>
+      </c>
+      <c r="U2" t="s">
+        <v>162</v>
+      </c>
+      <c r="V2" t="s">
+        <v>163</v>
+      </c>
+      <c r="W2" t="s">
+        <v>164</v>
+      </c>
+      <c r="X2" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>165</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>133</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>167</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>168</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>167</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>168</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>168</v>
+      </c>
+      <c r="AJ2">
+        <v>1000</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>170</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>172</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>173</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>174</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AR2" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="AS2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>175</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AV2" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AZ2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>96</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{268D7402-2FCA-45EE-8778-43C931A45300}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{D7041574-6382-4D6D-9785-3ECBDC2FBCFB}"/>
+    <hyperlink ref="B2" r:id="rId3" xr:uid="{952C66E8-A120-4052-A57A-F0BC63477EC1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>